<commit_message>
Move and Inventory and Character
</commit_message>
<xml_diff>
--- a/Solo/Assets/4.Arts/Table/ItemMonsterTable.xlsx
+++ b/Solo/Assets/4.Arts/Table/ItemMonsterTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +109,22 @@
   </si>
   <si>
     <t>BeginnerShield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -478,10 +494,12 @@
     <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +512,20 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -508,8 +538,20 @@
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -522,8 +564,20 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>100000</v>
       </c>
@@ -536,8 +590,20 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -550,8 +616,20 @@
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>200000</v>
       </c>
@@ -564,8 +642,20 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>100</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>210000</v>
       </c>
@@ -578,8 +668,20 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>220000</v>
       </c>
@@ -591,6 +693,18 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>